<commit_message>
nuevo requerimiento trabajado cobro de efectivo de notas de remision por parte del cajero
</commit_message>
<xml_diff>
--- a/files/documents/xls/prueba.xlsx
+++ b/files/documents/xls/prueba.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB2C648-A5C9-4BB4-8188-EAD6E7640844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C9DC12-FBA3-4D9A-ABBD-00DE9DFC266C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C91B417E-842A-4C51-87D0-592099401448}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>nombre de docente 5</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>kjhk</t>
+  </si>
+  <si>
+    <t>ff</t>
   </si>
 </sst>
 </file>
@@ -521,7 +524,7 @@
   <dimension ref="A1:Q6001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A9"/>
+      <selection activeCell="A6" sqref="A6:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,6 +572,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="7">
+        <f>SUM(E6:E15)</f>
         <v>96789</v>
       </c>
       <c r="C4" s="4"/>
@@ -764,8 +768,17 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="6">
+        <f>SUM(E6:E15)</f>
+        <v>96789</v>
+      </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" s="2"/>

</xml_diff>